<commit_message>
DDL + DML + requests
</commit_message>
<xml_diff>
--- a/Физическая модель.xlsx
+++ b/Физическая модель.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Department</t>
   </si>
@@ -219,12 +219,6 @@
     <t xml:space="preserve">Название предмета</t>
   </si>
   <si>
-    <t xml:space="preserve">time </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Время проведения занятия</t>
-  </si>
-  <si>
     <t>Teacher</t>
   </si>
   <si>
@@ -238,6 +232,9 @@
   </si>
   <si>
     <t xml:space="preserve">Электронная почта преподователя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK -&gt; AcademicHistory(history_id)	</t>
   </si>
 </sst>
 </file>
@@ -294,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -317,15 +314,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -334,9 +324,6 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,7 +835,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B24" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B9" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1249,12 +1236,12 @@
       </c>
     </row>
     <row r="32" ht="15">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" ht="15">
       <c r="B33" s="2" t="s">
@@ -1318,17 +1305,17 @@
       <c r="D37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" ht="15">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" ht="15">
       <c r="B39" s="2" t="s">
@@ -1380,15 +1367,17 @@
       <c r="D42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="43" ht="15">
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
     </row>
     <row r="44" ht="15">
       <c r="B44" s="2" t="s">
@@ -1431,13 +1420,13 @@
       <c r="E46" s="4"/>
     </row>
     <row r="47" ht="15">
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -1459,38 +1448,38 @@
       </c>
     </row>
     <row r="49" ht="15">
-      <c r="B49" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="B49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" ht="15">
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="51" ht="15">
-      <c r="B51" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="B51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1499,137 +1488,64 @@
         <v>9</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" ht="15">
+      <c r="E52" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" ht="30">
       <c r="B53" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" ht="15">
-      <c r="B54" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" ht="30">
+      <c r="B54" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="55" ht="15">
       <c r="B55" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" ht="15">
-      <c r="B56" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" ht="15">
-      <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" ht="15">
-      <c r="B58" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" ht="15">
-      <c r="B59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" ht="30">
-      <c r="B60" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" ht="30">
-      <c r="B61" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" ht="15">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-    </row>
+    </row>
+    <row r="56" ht="15"/>
+    <row r="57" ht="15"/>
+    <row r="58" ht="15"/>
+    <row r="59" ht="15"/>
+    <row r="60" ht="30"/>
+    <row r="61" ht="30"/>
+    <row r="62" ht="15"/>
     <row r="63" ht="15">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1638,7 +1554,7 @@
     </row>
     <row r="67" ht="14.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="9">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B13:E13"/>
@@ -1648,8 +1564,6 @@
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B62:E62"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>